<commit_message>
Generalization of Photo ODE model, modelling of photochemical mechanisms other than two-photon water splitting, change of energy unit from kcal/mol to kJ/mol, addition of time resolved UV/Vis data and analysis
</commit_message>
<xml_diff>
--- a/Computational_Data/DE_Scan/DE_Scan_Energies.xlsx
+++ b/Computational_Data/DE_Scan/DE_Scan_Energies.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jacob/Documents/Water_Splitting/Two_Photon_Water_Splitting/Computational_Data/DE_Scan/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5D2A51-F3A3-DF49-8201-5C20141F0108}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="0" windowWidth="13020" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="19640" windowHeight="14060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
   <definedNames>
     <definedName name="energies" localSheetId="0">Sheet1!$B$14:$C$20</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,8 +28,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="energies.dat" type="6" refreshedVersion="0" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="energies.dat" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:Jacob:Documents:Water_Splitting:Two_Photon_Water_Splitting:Computational_Data:DE_Scan:J-Trans-Mono-H2O-T0-RuO-Scan-GPO:energies.dat" thousands=" ">
       <textFields count="2">
         <textField/>
@@ -43,12 +49,6 @@
     <t>SMD Energy (Hartree)</t>
   </si>
   <si>
-    <t>Gas Phase Energy (kcal/mol)</t>
-  </si>
-  <si>
-    <t>SMD Energy (kcal/mol)</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
@@ -86,12 +86,18 @@
   </si>
   <si>
     <t>structure_007.png</t>
+  </si>
+  <si>
+    <t>Gas Phase Energy (kJ/mol)</t>
+  </si>
+  <si>
+    <t>SMD Energy (kJ/mol)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -136,11 +142,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="energies" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="energies" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,53 +478,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2.77</v>
       </c>
@@ -518,30 +532,31 @@
         <v>-1629.683556</v>
       </c>
       <c r="C2">
-        <f>(B2-$B$2)*627.5095</f>
+        <f>(B2-$B$2)*2625.5</f>
         <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>-1630.0490120500001</v>
       </c>
       <c r="E2">
-        <f>(D2-$D$2)*627.5095</f>
+        <f>(D2-$D$2)*2625.5</f>
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>0.12</v>
       </c>
       <c r="H2">
+        <f>1.9</f>
         <v>1.9</v>
       </c>
       <c r="I2">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3.27</v>
       </c>
@@ -549,18 +564,18 @@
         <v>-1629.6751794500001</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="0">(B3-$B$2)*627.5095</f>
-        <v>5.2563647021410747</v>
+        <f t="shared" ref="C3:C8" si="0">(B3-$B$2)*2625.5</f>
+        <v>21.992632024648856</v>
       </c>
       <c r="D3" s="2">
         <v>-1630.0450363099999</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E8" si="1">(D3-$D$2)*627.5095</f>
-        <v>2.4948146196646013</v>
+        <f t="shared" ref="E3:E8" si="1">(D3-$D$2)*2625.5</f>
+        <v>10.438305370563171</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>0.12</v>
@@ -572,7 +587,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>A3+0.5</f>
         <v>3.77</v>
@@ -582,17 +597,17 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>2.8302686480453372</v>
+        <v>11.841845160022331</v>
       </c>
       <c r="D4" s="2">
         <v>-1630.0619169300001</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>-8.097934796329211</v>
+        <v>-33.881762439871181</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>0.12</v>
@@ -604,7 +619,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ref="A5:A8" si="2">A4+0.5</f>
         <v>4.2699999999999996</v>
@@ -614,17 +629,17 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>10.453856463087998</v>
+        <v>43.738939639698742</v>
       </c>
       <c r="D5" s="2">
         <v>-1630.0598158099999</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>-6.7794620356051505</v>
+        <v>-28.365271879519469</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>0.12</v>
@@ -636,7 +651,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>4.7699999999999996</v>
@@ -646,17 +661,17 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>5.8980935674045663</v>
+        <v>24.677625854621624</v>
       </c>
       <c r="D6" s="2">
         <v>-1630.0349033699999</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>8.8533307325623323</v>
+        <v>37.042339340428157</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>0.12</v>
@@ -668,7 +683,7 @@
         <v>-0.13</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>5.27</v>
@@ -678,17 +693,17 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>6.2340182280696279</v>
+        <v>26.083134769747403</v>
       </c>
       <c r="D7" s="2">
         <v>-1630.0354207099999</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>8.5286949678401136</v>
+        <v>35.684063170460718</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G7">
         <v>0.12</v>
@@ -700,7 +715,7 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>5.77</v>
@@ -710,17 +725,17 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>7.0061561176320177</v>
+        <v>29.313760009757402</v>
       </c>
       <c r="D8" s="2">
         <v>-1630.03517197</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>8.6847816808455729</v>
+        <v>36.337130040358034</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G8">
         <v>0.12</v>
@@ -732,7 +747,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="1"/>
     </row>
   </sheetData>

</xml_diff>